<commit_message>
added ability to use excel shites
</commit_message>
<xml_diff>
--- a/static/data/prayer_data.xlsx
+++ b/static/data/prayer_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedir\Documents\API\Project\read from excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kedir\Documents\API\Prayer-Time-Display-2\static\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C359BA-01FA-4517-8CCB-83C78EAC5C8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E23CF01-9BEF-4C00-B9BF-AFE29770BAF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{1E559511-15BE-4465-AE73-3E6DB6FC246C}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11430" activeTab="9" xr2:uid="{1E559511-15BE-4465-AE73-3E6DB6FC246C}"/>
   </bookViews>
   <sheets>
     <sheet name="May" sheetId="14" r:id="rId1"/>
@@ -1249,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{740D7ED7-3BF1-4E65-B676-1835815E9CA4}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8553,7 +8553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1BBC5E-A701-47A2-BF51-EEF1A7CCA6BE}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
@@ -10613,7 +10613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15FB120-5489-4C2A-81AB-A366FC8675CE}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection sqref="A1:M33"/>
     </sheetView>
   </sheetViews>

</xml_diff>